<commit_message>
Added CDWA, CDWA-Lite and CIDOC/CRM to the table
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian Santini\Desktop\DHDK\Tomasi_2020\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcan\OneDrive - Alma Mater Studiorum Università di Bologna\DHDK\Knowledge Organization and Digital Methods in the Cultural Heritage Domain\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B1F845-0B9E-476D-A726-FB4986C869DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20961A3-A4B0-4185-8E1B-8C4EF31B0805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>created_by</t>
   </si>
@@ -203,6 +203,78 @@
   </si>
   <si>
     <t>published_by</t>
+  </si>
+  <si>
+    <t>CDWA</t>
+  </si>
+  <si>
+    <t>4.1.3. Creator Identity</t>
+  </si>
+  <si>
+    <t>kept_at</t>
+  </si>
+  <si>
+    <t>21. CURRENT LOCATION</t>
+  </si>
+  <si>
+    <t>CDWA Lite</t>
+  </si>
+  <si>
+    <t>CIDOC/CRM</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:nameCreator&gt;</t>
+  </si>
+  <si>
+    <t>4.3. Creation Place/Original Location</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:locationName&gt;</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>4.2. Creation Date</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:earliestDate&gt;, &lt;cdwalite:latestDate&gt;</t>
+  </si>
+  <si>
+    <t>16. SUBJECT MATTER</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:subjectTerm&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P2_has_type&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P67_refers_to&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P94_was_created by&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P4_has_time-span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P11_had_participant&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P55_has_current_location&gt;</t>
+  </si>
+  <si>
+    <t>2.1. Classification Term</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:classification&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P129_is_about&gt;, &lt;crm:P62_depicts&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P148_is_component_of&gt;</t>
   </si>
 </sst>
 </file>
@@ -558,15 +630,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="131.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -585,8 +670,17 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -605,8 +699,17 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -625,8 +728,17 @@
       <c r="F3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -645,8 +757,17 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -665,8 +786,17 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -685,8 +815,17 @@
       <c r="F6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -705,8 +844,17 @@
       <c r="F7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -725,8 +873,17 @@
       <c r="F8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -742,8 +899,17 @@
       <c r="F9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -758,6 +924,32 @@
       </c>
       <c r="E10" t="s">
         <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Archival Metadata Standard alignment
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcan\OneDrive - Alma Mater Studiorum Università di Bologna\DHDK\Knowledge Organization and Digital Methods in the Cultural Heritage Domain\KO-LAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20961A3-A4B0-4185-8E1B-8C4EF31B0805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9B3F3-6A0A-46E6-A030-B3DC5BDA0DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>created_by</t>
   </si>
@@ -275,6 +275,54 @@
   </si>
   <si>
     <t>&lt;crm:P148_is_component_of&gt;</t>
+  </si>
+  <si>
+    <t>ISAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAD </t>
+  </si>
+  <si>
+    <t>Name of Creator</t>
+  </si>
+  <si>
+    <t>Publication note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existance and location of originals </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extent and medium of the unit of descr. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope and content </t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;origination&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;repository&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;geogname&gt; </t>
+  </si>
+  <si>
+    <t>&lt;unitdatestructured&gt;</t>
+  </si>
+  <si>
+    <t>&lt;physicdescset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scopecontent&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mainentanceagency&gt;</t>
   </si>
 </sst>
 </file>
@@ -312,10 +360,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -630,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,310 +695,386 @@
     <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60.42578125" customWidth="1"/>
+    <col min="11" max="11" width="43.140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="J7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="J8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="J9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="J10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="J11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
property has_title, contains_note and has_genre added + cleaner e/r model
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian Santini\Desktop\DHDK\Tomasi_2020\Project\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39A767D-6AD2-4F23-BD33-7B2561F89B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30D2DA7-930A-4FB0-9B8F-DAE1358D58CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="114">
   <si>
     <t>created_by</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>25X-28X: Edition, Imprint, Etc. Fields - 260 - Production, Publication, Distribution, Manufacture, and Copyright Notice (R) - $b Name of publisher</t>
-  </si>
-  <si>
-    <t>1.4.1.1 Agent Activity = Director</t>
-  </si>
-  <si>
-    <t>1.4.1.1 Agent Activity = Distributor</t>
   </si>
   <si>
     <t>has publisher/distributor</t>
@@ -168,9 +162,6 @@
     <t>1.2.1 Work/Variant Type</t>
   </si>
   <si>
-    <t>1.4.1 Agents</t>
-  </si>
-  <si>
     <t>issued_in</t>
   </si>
   <si>
@@ -320,6 +311,73 @@
   </si>
   <si>
     <t xml:space="preserve">3.1 Scope and content </t>
+  </si>
+  <si>
+    <t>contains_note</t>
+  </si>
+  <si>
+    <t>&lt;dc:description&gt;</t>
+  </si>
+  <si>
+    <t>7.7 Notes relating to the contents</t>
+  </si>
+  <si>
+    <t>50X-53X: Note Fields: Part 1 - 500 General Note</t>
+  </si>
+  <si>
+    <t>has other distinguishing characteristic</t>
+  </si>
+  <si>
+    <t>1.3.6 Content description</t>
+  </si>
+  <si>
+    <t>has_genre</t>
+  </si>
+  <si>
+    <t>7.1.2.1 Genre notes</t>
+  </si>
+  <si>
+    <t>3XX: Physical Description, Etc. Fields - 380 - Form Of Work</t>
+  </si>
+  <si>
+    <t>7.2.4.6 Other relationships</t>
+  </si>
+  <si>
+    <t>53X-59X: Note Fields: Part 2 - 561 Ownership And Custodial History</t>
+  </si>
+  <si>
+    <t>owner relationship</t>
+  </si>
+  <si>
+    <t>1.3.8.1 Custodial history</t>
+  </si>
+  <si>
+    <t>7.2.3 Bibliographic history of the resource</t>
+  </si>
+  <si>
+    <t>0.3 Sources of Information</t>
+  </si>
+  <si>
+    <t>has_title</t>
+  </si>
+  <si>
+    <t>&lt;dc:title&gt;</t>
+  </si>
+  <si>
+    <t>1.1 Title proper</t>
+  </si>
+  <si>
+    <t>20X-24X: Title and Title-Related Fields - 245 Title Statement - $a Title</t>
+  </si>
+  <si>
+    <t>has title</t>
+  </si>
+  <si>
+    <t>1.3.2 Title</t>
+  </si>
+  <si>
+    <t>1.4.1 Agents (e.g. Cast, Credits, Person,
+Organisation, etc.)</t>
   </si>
 </sst>
 </file>
@@ -676,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +746,7 @@
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="131.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
     <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -700,7 +758,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -718,343 +776,425 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
+      <c r="F3" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>91</v>
-      </c>
-      <c r="K5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="K14" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Alignement: has_title has been added for CDWA, CDWA-Lite and CIDOC/CRM. Theoretical model has been added.
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian Santini\Desktop\DHDK\Tomasi_2020\Project\KO-LAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/arcangelo_massari_studio_unibo_it/Documents/DHDK/Knowledge Organization and Digital Methods in the Cultural Heritage Domain/KO-LAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30D2DA7-930A-4FB0-9B8F-DAE1358D58CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="6_{7AB9147D-3871-47A1-906C-8CB0CCA600B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{669F5A7D-626F-4D93-86AB-D06ECCAEB3FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
   <si>
     <t>created_by</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>1.3.4 Year/Date of reference</t>
-  </si>
-  <si>
-    <t>subject</t>
   </si>
   <si>
     <t>1.4.3 Subject/Genre/Form terms</t>
@@ -378,6 +375,21 @@
   <si>
     <t>1.4.1 Agents (e.g. Cast, Credits, Person,
 Organisation, etc.)</t>
+  </si>
+  <si>
+    <t>has_subject</t>
+  </si>
+  <si>
+    <t>3. TITLES OR NAMES</t>
+  </si>
+  <si>
+    <t>title &lt;title&gt;, &lt;defitem&gt;, &lt;label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P102_has_title&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:title&gt;</t>
   </si>
 </sst>
 </file>
@@ -736,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +770,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -776,43 +788,52 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="J1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
         <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -831,22 +852,22 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -866,21 +887,27 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -895,22 +922,22 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,24 +960,24 @@
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -968,132 +995,138 @@
         <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
+      <c r="J9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1102,97 +1135,109 @@
     </row>
     <row r="12" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M14" s="1"/>
     </row>

</xml_diff>

<commit_message>
archival title genre notes added
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/arcangelo_massari_studio_unibo_it/Documents/DHDK/Knowledge Organization and Digital Methods in the Cultural Heritage Domain/KO-LAM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="6_{7AB9147D-3871-47A1-906C-8CB0CCA600B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7A04A59-0841-4131-B4D3-5EBC2940F3CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E14643-2824-4AA5-84D4-30B06C1EDFAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
     <t>created_by</t>
   </si>
@@ -383,13 +383,22 @@
     <t>3. TITLES OR NAMES</t>
   </si>
   <si>
-    <t>title &lt;title&gt;, &lt;defitem&gt;, &lt;label&gt;</t>
-  </si>
-  <si>
     <t>&lt;crm:P102_has_title&gt;</t>
   </si>
   <si>
     <t>&lt;cdwalite:title&gt;</t>
+  </si>
+  <si>
+    <t>1.2 Title</t>
+  </si>
+  <si>
+    <t>&lt;title&gt;, &lt;defitem&gt;, &lt;label&gt; (@level)</t>
+  </si>
+  <si>
+    <t>6.1 Note</t>
+  </si>
+  <si>
+    <t>&lt;filedesc&gt;</t>
   </si>
 </sst>
 </file>
@@ -772,9 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -851,14 +860,16 @@
         <v>114</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1094,10 +1105,10 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1157,8 +1168,12 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1227,7 +1242,7 @@
         <v>61</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
e_r model consistent layout and consistency in file names
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/arcangelo_massari_studio_unibo_it/Documents/DHDK/Knowledge Organization and Digital Methods in the Cultural Heritage Domain/KO-LAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E14643-2824-4AA5-84D4-30B06C1EDFAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C0E14643-2824-4AA5-84D4-30B06C1EDFAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFA4551E-6AB9-4745-8F63-B581452A8140}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,73 +35,170 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
+    <t>RELATIONS</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	ISBD</t>
+  </si>
+  <si>
+    <t>MARC21</t>
+  </si>
+  <si>
+    <t>FRBR</t>
+  </si>
+  <si>
+    <t>FIAF</t>
+  </si>
+  <si>
+    <t>CDWA</t>
+  </si>
+  <si>
+    <t>CDWA Lite</t>
+  </si>
+  <si>
+    <t>CIDOC/CRM</t>
+  </si>
+  <si>
+    <t>ISAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAD </t>
+  </si>
+  <si>
+    <t>has_title</t>
+  </si>
+  <si>
+    <t>&lt;dc:title&gt;</t>
+  </si>
+  <si>
+    <t>1.1 Title proper</t>
+  </si>
+  <si>
+    <t>20X-24X: Title and Title-Related Fields - 245 Title Statement - $a Title</t>
+  </si>
+  <si>
+    <t>has title</t>
+  </si>
+  <si>
+    <t>1.3.2 Title</t>
+  </si>
+  <si>
+    <t>3. TITLES OR NAMES</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:title&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P102_has_title&gt;</t>
+  </si>
+  <si>
+    <t>1.2 Title</t>
+  </si>
+  <si>
+    <t>&lt;title&gt;, &lt;defitem&gt;, &lt;label&gt; (@level)</t>
+  </si>
+  <si>
     <t>created_by</t>
   </si>
   <si>
+    <t>&lt;dc:creator&gt;</t>
+  </si>
+  <si>
+    <t>1.4 Statement of responsibility</t>
+  </si>
+  <si>
+    <t>1XX: Main Entry Fields - 100 - Main Entry - $a Personal Name</t>
+  </si>
+  <si>
+    <t>has statement of responsibility</t>
+  </si>
+  <si>
+    <t>1.4.1 Agents (e.g. Cast, Credits, Person,
+Organisation, etc.)</t>
+  </si>
+  <si>
+    <t>4.1.3. Creator Identity</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:nameCreator&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P94_was_created by&gt;</t>
+  </si>
+  <si>
+    <t>2.1 Name of Creator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;origination&gt; </t>
+  </si>
+  <si>
     <t>has_contributor</t>
   </si>
   <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	ISBD</t>
-  </si>
-  <si>
-    <t>MARC21</t>
-  </si>
-  <si>
-    <t>FRBR</t>
-  </si>
-  <si>
-    <t>FIAF</t>
-  </si>
-  <si>
-    <t>&lt;dc:creator&gt;</t>
-  </si>
-  <si>
-    <t>1.4 Statement of responsibility</t>
-  </si>
-  <si>
-    <t>1XX: Main Entry Fields - 100 - Main Entry - $a Personal Name</t>
-  </si>
-  <si>
-    <t>has statement of responsibility</t>
-  </si>
-  <si>
     <t>&lt;dc:contributor&gt;</t>
   </si>
   <si>
     <t>70X-75X - Added Entry Fields - General Information - 700 Personal Name - 710 Corporate Name</t>
   </si>
   <si>
+    <t>&lt;crm:P11_had_participant&gt;</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>published_by</t>
+  </si>
+  <si>
     <t>&lt;dc:publisher&gt;</t>
   </si>
   <si>
+    <t>4.2 Name of Publisher</t>
+  </si>
+  <si>
     <t>25X-28X: Edition, Imprint, Etc. Fields - 260 - Production, Publication, Distribution, Manufacture, and Copyright Notice (R) - $b Name of publisher</t>
   </si>
   <si>
     <t>has publisher/distributor</t>
   </si>
   <si>
+    <t>5.4 Publication note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;repository&gt; </t>
+  </si>
+  <si>
+    <t>has_place_of_creation</t>
+  </si>
+  <si>
     <t>&lt;dc:coverage&gt;</t>
   </si>
   <si>
+    <t>4.1 Place of publication, production and/or distribution</t>
+  </si>
+  <si>
     <t>25X-28X: Edition, Imprint, Etc. Fields - 264 - Production, Publication, Distribution, Manufacture, and Copyright Notice (R) - $a Place of production</t>
   </si>
   <si>
-    <t>4.1 Place of publication, production and/or distribution</t>
-  </si>
-  <si>
-    <t>4.2 Name of Publisher</t>
-  </si>
-  <si>
     <t>has place of publication/distribution</t>
   </si>
   <si>
     <t xml:space="preserve">1.3.3 Country of reference </t>
   </si>
   <si>
-    <t>has_place_of_creation</t>
+    <t>4.3. Creation Place/Original Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1 Existance and location of originals </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;geogname&gt; </t>
+  </si>
+  <si>
+    <t>created_in</t>
   </si>
   <si>
     <t>&lt;dc:date&gt;</t>
@@ -119,26 +216,119 @@
     <t>1.3.4 Year/Date of reference</t>
   </si>
   <si>
-    <t>1.4.3 Subject/Genre/Form terms</t>
+    <t>4.2. Creation Date</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:earliestDate&gt;, &lt;cdwalite:latestDate&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P4_has_time-span&gt;</t>
+  </si>
+  <si>
+    <t>1.3 Date</t>
+  </si>
+  <si>
+    <t>&lt;unitdatestructured&gt;</t>
+  </si>
+  <si>
+    <t>has_type</t>
+  </si>
+  <si>
+    <t>&lt;dc:type&gt;</t>
+  </si>
+  <si>
+    <t>0.1 Content Form</t>
+  </si>
+  <si>
+    <t>3XX: Physical Description, Etc. Fields - 336 - Content Type</t>
+  </si>
+  <si>
+    <t>has form of work</t>
+  </si>
+  <si>
+    <t>1.2.1 Work/Variant Type</t>
+  </si>
+  <si>
+    <t>2.1. Classification Term</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:classification&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P2_has_type&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 Extent and medium of the unit of descr. </t>
+  </si>
+  <si>
+    <t>&lt;physicdescset&gt;</t>
+  </si>
+  <si>
+    <t>contains_note</t>
+  </si>
+  <si>
+    <t>&lt;dc:description&gt;</t>
+  </si>
+  <si>
+    <t>7.7 Notes relating to the contents</t>
+  </si>
+  <si>
+    <t>50X-53X: Note Fields: Part 1 - 500 General Note</t>
+  </si>
+  <si>
+    <t>has other distinguishing characteristic</t>
+  </si>
+  <si>
+    <t>1.3.6 Content description</t>
+  </si>
+  <si>
+    <t>6.1 Note</t>
+  </si>
+  <si>
+    <t>&lt;filedesc&gt;</t>
+  </si>
+  <si>
+    <t>has_subject</t>
+  </si>
+  <si>
+    <t>&lt;dc:subject&gt;</t>
   </si>
   <si>
     <t>7.10.2 Note providing a summary</t>
   </si>
   <si>
-    <t>&lt;dc:subject&gt;</t>
-  </si>
-  <si>
-    <t>&lt;dc:type&gt;</t>
+    <t>6XX: Subject Access Fields</t>
   </si>
   <si>
     <t>has summarization of
 content</t>
   </si>
   <si>
-    <t>6XX: Subject Access Fields</t>
-  </si>
-  <si>
-    <t>created_in</t>
+    <t>1.4.3 Subject/Genre/Form terms</t>
+  </si>
+  <si>
+    <t>16. SUBJECT MATTER</t>
+  </si>
+  <si>
+    <t>&lt;cdwalite:subjectTerm&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crm:P129_is_about&gt;, &lt;crm:P62_depicts&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1 Scope and content </t>
+  </si>
+  <si>
+    <t>&lt;scopecontent&gt;</t>
+  </si>
+  <si>
+    <t>has_genre</t>
+  </si>
+  <si>
+    <t>7.1.2.1 Genre notes</t>
+  </si>
+  <si>
+    <t>3XX: Physical Description, Etc. Fields - 380 - Form Of Work</t>
   </si>
   <si>
     <t>relates_to</t>
@@ -147,19 +337,25 @@
     <t>&lt;dc:relation&gt;</t>
   </si>
   <si>
+    <t>7.2.4.6 Other relationships</t>
+  </si>
+  <si>
     <t>53X-59X: Note Fields: Part 2 - 580 Linking Entry Complexity Notes</t>
   </si>
   <si>
+    <t>context for the work</t>
+  </si>
+  <si>
+    <t>1.4.4 Other relationships</t>
+  </si>
+  <si>
+    <t>&lt;crm:P67_refers_to&gt;</t>
+  </si>
+  <si>
+    <t>issued_in</t>
+  </si>
+  <si>
     <t>&lt;dc:isPartOf&gt;</t>
-  </si>
-  <si>
-    <t>1.4.4 Other relationships</t>
-  </si>
-  <si>
-    <t>1.2.1 Work/Variant Type</t>
-  </si>
-  <si>
-    <t>issued_in</t>
   </si>
   <si>
     <t>6.1 Title proper of a series or multipart monographic
@@ -169,236 +365,40 @@
     <t>76X-78X: Linking Entry Fields - 760 Main Series Entry</t>
   </si>
   <si>
-    <t>context for the work</t>
-  </si>
-  <si>
-    <t>3XX: Physical Description, Etc. Fields - 336 - Content Type</t>
-  </si>
-  <si>
-    <t>0.1 Content Form</t>
-  </si>
-  <si>
-    <t>has form of work</t>
-  </si>
-  <si>
     <t>has edition/issue designation</t>
   </si>
   <si>
-    <t>RELATIONS</t>
-  </si>
-  <si>
-    <t>has_type</t>
-  </si>
-  <si>
-    <t>published_by</t>
-  </si>
-  <si>
-    <t>CDWA</t>
-  </si>
-  <si>
-    <t>4.1.3. Creator Identity</t>
+    <t>0.3 Sources of Information</t>
+  </si>
+  <si>
+    <t>&lt;crm:P148_is_component_of&gt;</t>
   </si>
   <si>
     <t>kept_at</t>
   </si>
   <si>
+    <t>7.2.3 Bibliographic history of the resource</t>
+  </si>
+  <si>
+    <t>53X-59X: Note Fields: Part 2 - 561 Ownership And Custodial History</t>
+  </si>
+  <si>
+    <t>owner relationship</t>
+  </si>
+  <si>
+    <t>1.3.8.1 Custodial history</t>
+  </si>
+  <si>
     <t>21. CURRENT LOCATION</t>
   </si>
   <si>
-    <t>CDWA Lite</t>
-  </si>
-  <si>
-    <t>CIDOC/CRM</t>
-  </si>
-  <si>
-    <t>&lt;cdwalite:nameCreator&gt;</t>
-  </si>
-  <si>
-    <t>4.3. Creation Place/Original Location</t>
-  </si>
-  <si>
     <t>&lt;cdwalite:locationName&gt;</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>4.2. Creation Date</t>
-  </si>
-  <si>
-    <t>&lt;cdwalite:earliestDate&gt;, &lt;cdwalite:latestDate&gt;</t>
-  </si>
-  <si>
-    <t>16. SUBJECT MATTER</t>
-  </si>
-  <si>
-    <t>&lt;cdwalite:subjectTerm&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P2_has_type&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P67_refers_to&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P94_was_created by&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P4_has_time-span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P11_had_participant&gt;</t>
-  </si>
-  <si>
     <t>&lt;crm:P55_has_current_location&gt;</t>
   </si>
   <si>
-    <t>2.1. Classification Term</t>
-  </si>
-  <si>
-    <t>&lt;cdwalite:classification&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P129_is_about&gt;, &lt;crm:P62_depicts&gt;</t>
-  </si>
-  <si>
-    <t>&lt;crm:P148_is_component_of&gt;</t>
-  </si>
-  <si>
-    <t>ISAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;origination&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;repository&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;geogname&gt; </t>
-  </si>
-  <si>
-    <t>&lt;unitdatestructured&gt;</t>
-  </si>
-  <si>
-    <t>&lt;physicdescset&gt;</t>
-  </si>
-  <si>
-    <t>&lt;scopecontent&gt;</t>
-  </si>
-  <si>
     <t>&lt;mainentanceagency&gt;</t>
-  </si>
-  <si>
-    <t>2.1 Name of Creator</t>
-  </si>
-  <si>
-    <t>5.4 Publication note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.1 Existance and location of originals </t>
-  </si>
-  <si>
-    <t>1.3 Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5 Extent and medium of the unit of descr. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1 Scope and content </t>
-  </si>
-  <si>
-    <t>contains_note</t>
-  </si>
-  <si>
-    <t>&lt;dc:description&gt;</t>
-  </si>
-  <si>
-    <t>7.7 Notes relating to the contents</t>
-  </si>
-  <si>
-    <t>50X-53X: Note Fields: Part 1 - 500 General Note</t>
-  </si>
-  <si>
-    <t>has other distinguishing characteristic</t>
-  </si>
-  <si>
-    <t>1.3.6 Content description</t>
-  </si>
-  <si>
-    <t>has_genre</t>
-  </si>
-  <si>
-    <t>7.1.2.1 Genre notes</t>
-  </si>
-  <si>
-    <t>3XX: Physical Description, Etc. Fields - 380 - Form Of Work</t>
-  </si>
-  <si>
-    <t>7.2.4.6 Other relationships</t>
-  </si>
-  <si>
-    <t>53X-59X: Note Fields: Part 2 - 561 Ownership And Custodial History</t>
-  </si>
-  <si>
-    <t>owner relationship</t>
-  </si>
-  <si>
-    <t>1.3.8.1 Custodial history</t>
-  </si>
-  <si>
-    <t>7.2.3 Bibliographic history of the resource</t>
-  </si>
-  <si>
-    <t>0.3 Sources of Information</t>
-  </si>
-  <si>
-    <t>has_title</t>
-  </si>
-  <si>
-    <t>&lt;dc:title&gt;</t>
-  </si>
-  <si>
-    <t>1.1 Title proper</t>
-  </si>
-  <si>
-    <t>20X-24X: Title and Title-Related Fields - 245 Title Statement - $a Title</t>
-  </si>
-  <si>
-    <t>has title</t>
-  </si>
-  <si>
-    <t>1.3.2 Title</t>
-  </si>
-  <si>
-    <t>1.4.1 Agents (e.g. Cast, Credits, Person,
-Organisation, etc.)</t>
-  </si>
-  <si>
-    <t>has_subject</t>
-  </si>
-  <si>
-    <t>3. TITLES OR NAMES</t>
-  </si>
-  <si>
-    <t>&lt;crm:P102_has_title&gt;</t>
-  </si>
-  <si>
-    <t>&lt;cdwalite:title&gt;</t>
-  </si>
-  <si>
-    <t>1.2 Title</t>
-  </si>
-  <si>
-    <t>&lt;title&gt;, &lt;defitem&gt;, &lt;label&gt; (@level)</t>
-  </si>
-  <si>
-    <t>6.1 Note</t>
-  </si>
-  <si>
-    <t>&lt;filedesc&gt;</t>
   </si>
 </sst>
 </file>
@@ -781,9 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -804,480 +804,480 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="K7" s="4" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>100</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed data description duplicated
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -782,8 +782,8 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9:K9"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
minimum edit for prefixes
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian Santini\Desktop\KO-LAM1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian Santini\Desktop\DHDK\Tomasi_2020\Project\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D7B5C-0DB9-44F7-AEC3-67F3D64E3AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EED047-F7DA-47FD-8A6B-64ECB130E432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="120">
   <si>
     <t>created_by</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>&lt;rdai:containedInItem.en&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rdai:categoryOfItem.en&gt;</t>
   </si>
 </sst>
 </file>
@@ -775,7 +778,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E13" sqref="E13"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1056,7 @@
         <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added EAC & ISAAR
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676F84AF-6408-47B8-9769-46DCDAA5CC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341A2287-313D-41F4-8B84-BDE7D6590A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="135">
   <si>
     <t>created_by</t>
   </si>
@@ -397,6 +397,48 @@
   </si>
   <si>
     <t>&lt;controlaccess&gt;&lt;persname&gt;</t>
+  </si>
+  <si>
+    <t>ISAAR</t>
+  </si>
+  <si>
+    <t>&lt;entityType&gt;</t>
+  </si>
+  <si>
+    <t>5.1.1 Type of entity</t>
+  </si>
+  <si>
+    <t>5.1.2 Authorized form(s) of name</t>
+  </si>
+  <si>
+    <t>&lt;nameEntry&gt;</t>
+  </si>
+  <si>
+    <t>&lt;place&gt;</t>
+  </si>
+  <si>
+    <t>5.2.3 Places</t>
+  </si>
+  <si>
+    <t>&lt;existDates&gt;</t>
+  </si>
+  <si>
+    <t>5.2.1 Dates of existence</t>
+  </si>
+  <si>
+    <t>5.2.8 General context</t>
+  </si>
+  <si>
+    <t>&lt;generalContext&gt;</t>
+  </si>
+  <si>
+    <t>5.3 Relationships area</t>
+  </si>
+  <si>
+    <t>&lt;relations&gt;</t>
+  </si>
+  <si>
+    <t>EAC-CPF</t>
   </si>
 </sst>
 </file>
@@ -777,11 +819,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -797,10 +839,11 @@
     <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="60.42578125" customWidth="1"/>
     <col min="11" max="11" width="43.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="33.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -834,8 +877,14 @@
       <c r="K1" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -869,8 +918,14 @@
       <c r="K2" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="L2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -904,8 +959,14 @@
       <c r="K3" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -939,8 +1000,14 @@
       <c r="K4" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -974,8 +1041,14 @@
       <c r="K5" s="4" t="s">
         <v>116</v>
       </c>
+      <c r="L5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1009,8 +1082,14 @@
       <c r="K6" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="L6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1044,8 +1123,14 @@
       <c r="K7" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="L7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -1079,8 +1164,14 @@
       <c r="K8" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="L8" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>70</v>
       </c>
@@ -1108,8 +1199,14 @@
       <c r="K9" s="4" t="s">
         <v>119</v>
       </c>
+      <c r="L9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>83</v>
       </c>
@@ -1143,8 +1240,14 @@
       <c r="K10" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="L10" t="s">
+        <v>130</v>
+      </c>
+      <c r="M10" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1172,8 +1275,14 @@
       <c r="K11" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1207,8 +1316,14 @@
       <c r="K12" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="L12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1242,8 +1357,14 @@
       <c r="K13" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="L13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -1275,8 +1396,14 @@
       <c r="K14" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="L14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 5.x.x problem in m_align
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{341A2287-313D-41F4-8B84-BDE7D6590A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{48189018-027A-4772-8453-D1A71C0B1A32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DECAB0A-ABE4-456C-BB93-DADFC8B92A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>&lt;unittitle&gt;</t>
   </si>
   <si>
-    <t>5.1.2 Authorized form(s) of name</t>
-  </si>
-  <si>
     <t>&lt;nameEntry&gt;</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>&lt;controlaccess&gt;&lt;geogname&gt;</t>
   </si>
   <si>
-    <t>5.2.3 Places</t>
-  </si>
-  <si>
     <t>&lt;place&gt;</t>
   </si>
   <si>
@@ -251,9 +245,6 @@
     <t>&lt;unitdatestructured&gt;</t>
   </si>
   <si>
-    <t>5.2.1 Dates of existence</t>
-  </si>
-  <si>
     <t>&lt;existDates&gt;</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
     <t>&lt;physdesc&gt;, &lt;physdescstructured&gt;</t>
   </si>
   <si>
-    <t>5.1.1 Type of entity</t>
-  </si>
-  <si>
     <t>&lt;entityType&gt;</t>
   </si>
   <si>
@@ -344,9 +332,6 @@
     <t>&lt;scopecontent&gt;</t>
   </si>
   <si>
-    <t>5.2.8 General context</t>
-  </si>
-  <si>
     <t>&lt;generalContext&gt;</t>
   </si>
   <si>
@@ -384,9 +369,6 @@
   </si>
   <si>
     <t>&lt;crm:P67_refers_to&gt;</t>
-  </si>
-  <si>
-    <t>5.3 Relationships area</t>
   </si>
   <si>
     <t>&lt;relations&gt;</t>
@@ -439,13 +421,31 @@
   </si>
   <si>
     <t>&lt;mainentanceagency&gt;</t>
+  </si>
+  <si>
+    <t>1.2 Authorized form(s) of name</t>
+  </si>
+  <si>
+    <t>2.3 Places</t>
+  </si>
+  <si>
+    <t>2.1 Dates of existence</t>
+  </si>
+  <si>
+    <t>1.1 Type of entity</t>
+  </si>
+  <si>
+    <t>2.8 General context</t>
+  </si>
+  <si>
+    <t>3 Relationships area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,7 +507,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -822,11 +822,11 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -843,7 +843,7 @@
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -919,493 +919,493 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="48.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>36</v>
+      <c r="I4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="4" t="s">
+    <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>36</v>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="52.5" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="4" t="s">
+    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>36</v>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="4" t="s">
+    <row r="7" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M6" t="s">
+      <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="4" t="s">
+    <row r="8" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="M7" t="s">
+      <c r="C8" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="4" t="s">
+    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L8" t="s">
+      <c r="C9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M8" t="s">
+      <c r="D9" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="L9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" t="s">
-        <v>36</v>
+      <c r="E10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" t="s">
+        <v>133</v>
+      </c>
+      <c r="M10" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="4" t="s">
+    <row r="11" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L10" t="s">
+      <c r="E11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="M10" t="s">
+      <c r="F11" s="4" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31.5" customHeight="1">
+    <row r="12" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="G12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="J12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="4" t="s">
+    </row>
+    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="G13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="5" t="s">
+    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>36</v>
+      <c r="I14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ontologies for archive
</commit_message>
<xml_diff>
--- a/metadata_alignment.xlsx
+++ b/metadata_alignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margherita\Desktop\KNOWLEDGE ORGANIZATION\KO-LAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DECAB0A-ABE4-456C-BB93-DADFC8B92A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ECC1D5-EBC6-4223-BC33-A212001A2C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B65A268-4AFC-4E99-A273-FDD551894291}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
   <si>
     <t>RELATIONS</t>
   </si>
@@ -439,6 +439,48 @@
   </si>
   <si>
     <t>3 Relationships area</t>
+  </si>
+  <si>
+    <t>OAD</t>
+  </si>
+  <si>
+    <t>EAC-CPF (Ontology)</t>
+  </si>
+  <si>
+    <t>oad:title</t>
+  </si>
+  <si>
+    <t>oad:isProducedBy</t>
+  </si>
+  <si>
+    <t>oad:hasPublicationNote</t>
+  </si>
+  <si>
+    <t>eac-cpf:place</t>
+  </si>
+  <si>
+    <t>oad:date</t>
+  </si>
+  <si>
+    <t>eac-cpf:existDates</t>
+  </si>
+  <si>
+    <t>oad:hasExtentType</t>
+  </si>
+  <si>
+    <t>oad:note</t>
+  </si>
+  <si>
+    <t>oad:scopeAndContent</t>
+  </si>
+  <si>
+    <t>eac-cpf:generalContext</t>
+  </si>
+  <si>
+    <t>eac-cpf:involves</t>
+  </si>
+  <si>
+    <t>eac-cpf:named</t>
   </si>
 </sst>
 </file>
@@ -819,11 +861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FA8767-0E79-410F-965B-77A761AD4A61}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -841,9 +883,11 @@
     <col min="11" max="11" width="43.140625" customWidth="1"/>
     <col min="12" max="12" width="33.7109375" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -883,8 +927,14 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -924,8 +974,14 @@
       <c r="M2" t="s">
         <v>23</v>
       </c>
+      <c r="N2" t="s">
+        <v>137</v>
+      </c>
+      <c r="O2" t="s">
+        <v>148</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -965,8 +1021,14 @@
       <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="N3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1006,8 +1068,14 @@
       <c r="M4" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1047,8 +1115,14 @@
       <c r="M5" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="N5" t="s">
+        <v>139</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -1088,8 +1162,11 @@
       <c r="M6" t="s">
         <v>58</v>
       </c>
+      <c r="O6" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
@@ -1129,8 +1206,14 @@
       <c r="M7" t="s">
         <v>70</v>
       </c>
+      <c r="N7" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -1170,8 +1253,14 @@
       <c r="M8" t="s">
         <v>81</v>
       </c>
+      <c r="N8" t="s">
+        <v>143</v>
+      </c>
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
@@ -1205,8 +1294,14 @@
       <c r="M9" t="s">
         <v>35</v>
       </c>
+      <c r="N9" t="s">
+        <v>144</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>89</v>
       </c>
@@ -1246,8 +1341,14 @@
       <c r="M10" t="s">
         <v>99</v>
       </c>
+      <c r="N10" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>100</v>
       </c>
@@ -1281,8 +1382,14 @@
       <c r="M11" t="s">
         <v>35</v>
       </c>
+      <c r="N11" t="s">
+        <v>145</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>105</v>
       </c>
@@ -1322,8 +1429,11 @@
       <c r="M12" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="O12" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>113</v>
       </c>
@@ -1363,8 +1473,14 @@
       <c r="M13" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>121</v>
       </c>
@@ -1404,8 +1520,14 @@
       <c r="M14" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>

</xml_diff>